<commit_message>
changes to flight selectors with screen scraping
</commit_message>
<xml_diff>
--- a/P2_Performer/Results/03-29-2023/Fred Smith - Boise, Idaho, United States of America.xlsx
+++ b/P2_Performer/Results/03-29-2023/Fred Smith - Boise, Idaho, United States of America.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\Results\03-29-2023\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE958811-8531-4236-B039-11767B893ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="3108" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,15 +77,15 @@
     <t>Airline</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Schedule</t>
   </si>
   <si>
     <t>Duration</t>
   </si>
   <si>
+    <t>Cost / ticket</t>
+  </si>
+  <si>
     <t>Morrison Center for the Performing Arts</t>
   </si>
   <si>
@@ -146,15 +152,6 @@
     <t>Hotel 43</t>
   </si>
   <si>
-    <t>United</t>
-  </si>
-  <si>
-    <t>6:00 AM – 4:36 PM</t>
-  </si>
-  <si>
-    <t>12 hr 36 min</t>
-  </si>
-  <si>
     <t>AlaskaOperated by Horizon Air as Alaska Horizon</t>
   </si>
   <si>
@@ -162,12 +159,21 @@
   </si>
   <si>
     <t>14 hr 26 min</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>7:43 AM – 12:45 PM</t>
+  </si>
+  <si>
+    <t>7 hr 2 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -858,21 +864,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -900,9 +903,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1217,18 +1223,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1248,10 +1254,10 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1263,11 +1269,11 @@
       <c r="C2" s="12">
         <v>6</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="42">
         <f>PRODUCT(B2,C2)</f>
         <v>1962</v>
       </c>
-      <c r="E2" s="46"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -1279,11 +1285,11 @@
       <c r="C3" s="8">
         <v>6</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="42">
         <f t="shared" ref="D3:D4" si="0">PRODUCT(B3,C3)</f>
         <v>1830</v>
       </c>
-      <c r="E3" s="46"/>
+      <c r="E3" s="43"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
@@ -1295,78 +1301,78 @@
       <c r="C4" s="14">
         <v>6</v>
       </c>
-      <c r="D4" s="52">
+      <c r="D4" s="49">
         <f t="shared" si="0"/>
         <v>1962</v>
       </c>
-      <c r="E4" s="53"/>
+      <c r="E4" s="50"/>
     </row>
     <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="31" t="s">
+      <c r="E5" s="29" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="12" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="60">
-        <v>432</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="14" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="61">
-        <v>439</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
     </row>
     <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -1405,34 +1411,34 @@
       <c r="A13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="58"/>
     </row>
     <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -1655,6 +1661,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
@@ -1669,11 +1680,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>